<commit_message>
IT WORKS!!! but almost everything is commented out -_-
</commit_message>
<xml_diff>
--- a/Cryptography/texts/hill/decoded/texts.xlsx
+++ b/Cryptography/texts/hill/decoded/texts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juro\source\repos\KryptoImGui\KryptoImGui\texts\hill\decoded\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juro\source\repos\Cryptography\Cryptography\texts\hill\decoded\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E396F018-E027-44B4-A25E-1E30FA6AC1C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8178D1AC-7C4F-4304-90A8-FE13966D99F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -308,10 +308,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -597,8 +597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:Z41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -788,16 +788,16 @@
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="K6" s="8" t="s">
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="K6" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -1031,22 +1031,22 @@
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="M14" s="6"/>
@@ -1145,17 +1145,17 @@
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
       <c r="M18" s="6"/>
-      <c r="N18" s="8" t="s">
+      <c r="N18" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="O18" s="8"/>
-      <c r="P18" s="8"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19">
@@ -1232,17 +1232,17 @@
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
       <c r="M22" s="6"/>
-      <c r="N22" s="8" t="s">
+      <c r="N22" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="O22" s="8"/>
-      <c r="P22" s="8"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="7"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23">
@@ -1310,17 +1310,17 @@
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
       <c r="M26" s="6"/>
-      <c r="N26" s="8" t="s">
+      <c r="N26" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="O26" s="8"/>
-      <c r="P26" s="8"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="7"/>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27">
@@ -1397,17 +1397,17 @@
       <c r="T29" s="1"/>
     </row>
     <row r="30" spans="1:20" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
       <c r="M30" s="6"/>
-      <c r="N30" s="8" t="s">
+      <c r="N30" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="O30" s="8"/>
-      <c r="P30" s="8"/>
+      <c r="O30" s="7"/>
+      <c r="P30" s="7"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31">
@@ -1531,22 +1531,22 @@
       </c>
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
-      <c r="I34" s="7"/>
-      <c r="J34" s="7"/>
-      <c r="K34" s="7"/>
-      <c r="L34" s="7"/>
-      <c r="M34" s="7"/>
-      <c r="N34" s="7"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="8"/>
+      <c r="N34" s="8"/>
       <c r="O34" s="5"/>
       <c r="P34" s="5"/>
     </row>
@@ -1946,11 +1946,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="A13:N13"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A22:C22"/>
     <mergeCell ref="A34:N34"/>
     <mergeCell ref="A30:C30"/>
     <mergeCell ref="N18:P18"/>
@@ -1958,6 +1953,11 @@
     <mergeCell ref="N26:P26"/>
     <mergeCell ref="N30:P30"/>
     <mergeCell ref="A26:C26"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="A13:N13"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A22:C22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2141,16 +2141,16 @@
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="K6" s="8" t="s">
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="K6" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -2366,22 +2366,22 @@
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="M14" s="6"/>
@@ -2480,17 +2480,17 @@
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
       <c r="M18" s="6"/>
-      <c r="N18" s="8" t="s">
+      <c r="N18" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="O18" s="8"/>
-      <c r="P18" s="8"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19">
@@ -2558,17 +2558,17 @@
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
       <c r="M22" s="6"/>
-      <c r="N22" s="8" t="s">
+      <c r="N22" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="O22" s="8"/>
-      <c r="P22" s="8"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="7"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23">
@@ -2636,17 +2636,17 @@
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
       <c r="M26" s="6"/>
-      <c r="N26" s="8" t="s">
+      <c r="N26" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="O26" s="8"/>
-      <c r="P26" s="8"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="7"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27">
@@ -2714,17 +2714,17 @@
       </c>
     </row>
     <row r="30" spans="1:16" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
       <c r="M30" s="6"/>
-      <c r="N30" s="8" t="s">
+      <c r="N30" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="O30" s="8"/>
-      <c r="P30" s="8"/>
+      <c r="O30" s="7"/>
+      <c r="P30" s="7"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31">
@@ -2820,22 +2820,22 @@
       </c>
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
-      <c r="I34" s="7"/>
-      <c r="J34" s="7"/>
-      <c r="K34" s="7"/>
-      <c r="L34" s="7"/>
-      <c r="M34" s="7"/>
-      <c r="N34" s="7"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="8"/>
+      <c r="N34" s="8"/>
       <c r="O34" s="5"/>
       <c r="P34" s="5"/>
     </row>
@@ -3193,6 +3193,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="N26:P26"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="N30:P30"/>
+    <mergeCell ref="A34:N34"/>
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="N22:P22"/>
     <mergeCell ref="F6:H6"/>
@@ -3200,11 +3205,6 @@
     <mergeCell ref="A13:N13"/>
     <mergeCell ref="A18:C18"/>
     <mergeCell ref="N18:P18"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="N26:P26"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="N30:P30"/>
-    <mergeCell ref="A34:N34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3378,16 +3378,16 @@
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="K6" s="8" t="s">
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="K6" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -3594,22 +3594,22 @@
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="M14" s="6"/>
@@ -3708,17 +3708,17 @@
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
       <c r="M18" s="6"/>
-      <c r="N18" s="8" t="s">
+      <c r="N18" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="O18" s="8"/>
-      <c r="P18" s="8"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19">
@@ -3786,17 +3786,17 @@
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
       <c r="M22" s="6"/>
-      <c r="N22" s="8" t="s">
+      <c r="N22" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="O22" s="8"/>
-      <c r="P22" s="8"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="7"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23">
@@ -3864,17 +3864,17 @@
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
       <c r="M26" s="6"/>
-      <c r="N26" s="8" t="s">
+      <c r="N26" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="O26" s="8"/>
-      <c r="P26" s="8"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="7"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27">
@@ -3942,17 +3942,17 @@
       </c>
     </row>
     <row r="30" spans="1:16" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
       <c r="M30" s="6"/>
-      <c r="N30" s="8" t="s">
+      <c r="N30" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="O30" s="8"/>
-      <c r="P30" s="8"/>
+      <c r="O30" s="7"/>
+      <c r="P30" s="7"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31">
@@ -4048,22 +4048,22 @@
       </c>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
-      <c r="I34" s="7"/>
-      <c r="J34" s="7"/>
-      <c r="K34" s="7"/>
-      <c r="L34" s="7"/>
-      <c r="M34" s="7"/>
-      <c r="N34" s="7"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="8"/>
+      <c r="N34" s="8"/>
       <c r="O34" s="5"/>
       <c r="P34" s="5"/>
     </row>
@@ -4400,6 +4400,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="N26:P26"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="N30:P30"/>
+    <mergeCell ref="A34:N34"/>
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="N22:P22"/>
     <mergeCell ref="F6:H6"/>
@@ -4407,11 +4412,6 @@
     <mergeCell ref="A13:N13"/>
     <mergeCell ref="A18:C18"/>
     <mergeCell ref="N18:P18"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="N26:P26"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="N30:P30"/>
-    <mergeCell ref="A34:N34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>